<commit_message>
branch works now. It was a buggy workbook that crashed the server for some reason
</commit_message>
<xml_diff>
--- a/test-files/additional-sheet-test-files/optimization-parameters-default.xlsx
+++ b/test-files/additional-sheet-test-files/optimization-parameters-default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" state="visible" r:id="rId2"/>
@@ -436,10 +436,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -577,38 +577,6 @@
         <v>0.1042</v>
       </c>
     </row>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1454,8 +1422,8 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Refactored import to retain all network sheets without changing the functionality of existing code. Created export constants for export tests
</commit_message>
<xml_diff>
--- a/test-files/additional-sheet-test-files/optimization-parameters-default.xlsx
+++ b/test-files/additional-sheet-test-files/optimization-parameters-default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" state="visible" r:id="rId2"/>
@@ -234,18 +234,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -301,7 +295,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,7 +312,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,27 +328,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1422,8 +1412,8 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1445,7 +1435,7 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="13" t="n">
+      <c r="B2" s="12" t="n">
         <v>0.002</v>
       </c>
     </row>
@@ -1461,7 +1451,7 @@
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="12" t="n">
         <v>100000000</v>
       </c>
     </row>
@@ -1469,7 +1459,7 @@
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="12" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -1477,7 +1467,7 @@
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="13" t="n">
+      <c r="B6" s="12" t="n">
         <v>100000000</v>
       </c>
     </row>
@@ -1485,7 +1475,7 @@
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="13" t="n">
+      <c r="B7" s="12" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -1652,8 +1642,8 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1964,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2692,660 +2682,660 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="5" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="n">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="n">
+      <c r="D1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="n">
+      <c r="E1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G1" s="3" t="n">
+      <c r="G1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="H1" s="3" t="n">
+      <c r="H1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J1" s="3" t="n">
+      <c r="J1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="K1" s="3" t="n">
+      <c r="K1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="L1" s="3" t="n">
+      <c r="L1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="M1" s="3" t="n">
+      <c r="M1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="N1" s="3"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>-0.1718</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="7" t="n">
         <v>-0.2792</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <v>-0.1752</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="6" t="n">
         <v>-0.6884</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>-0.2436</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="7" t="n">
         <v>0.1581</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="6" t="n">
         <v>-0.4253</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="5" t="n">
+      <c r="I2" s="8"/>
+      <c r="J2" s="6" t="n">
         <v>0.5682</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="K2" s="6" t="n">
         <v>0.1646</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="6" t="n">
         <v>-0.3202</v>
       </c>
-      <c r="M2" s="5" t="n">
+      <c r="M2" s="6" t="n">
         <v>-0.3888</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="5" t="n">
         <v>-1.3229</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="5" t="n">
         <v>-0.4236</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="5" t="n">
         <v>-1.8945</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="5" t="n">
         <v>-1.6929</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="5" t="n">
         <v>-2.2704</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="5" t="n">
         <v>-1.0939</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="5" t="n">
         <v>-1.3098</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="5" t="n">
         <v>-1.017</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="5" t="n">
         <v>-1.7106</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="5" t="n">
         <v>-1.7777</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="L3" s="5" t="n">
         <v>-1.9029</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="M3" s="5" t="n">
         <v>-1.3284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <v>-0.6685</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="5" t="n">
+      <c r="C4" s="7"/>
+      <c r="D4" s="6" t="n">
         <v>-0.4322</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>-0.1191</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="7" t="n">
         <v>-0.383</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="7" t="n">
         <v>0.2693</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="6" t="n">
         <v>-0.0757</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="6" t="n">
         <v>0.5975</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="5" t="n">
+      <c r="J4" s="8"/>
+      <c r="K4" s="6" t="n">
         <v>-0.3216</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="6" t="n">
         <v>0.0805</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="6" t="n">
         <v>0.4778</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <v>-0.3155</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="7" t="n">
         <v>1.4649</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="6" t="n">
         <v>-0.8029</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="6" t="n">
         <v>0.5141</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="7" t="n">
         <v>-0.7654</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="7" t="n">
         <v>-1.1456</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="6" t="n">
         <v>0.5096</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="6" t="n">
         <v>-0.2957</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="6" t="n">
         <v>-0.2257</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="6" t="n">
         <v>-0.9404</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="6" t="n">
         <v>-1.3326</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="6" t="n">
         <v>0.1689</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>0.9621</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="7" t="n">
         <v>-0.3518</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="6" t="n">
         <v>0.3101</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <v>-0.1589</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="7" t="n">
         <v>0.5869</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="7" t="n">
         <v>0.0341</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="6" t="n">
         <v>0.486</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="6" t="n">
         <v>0.4342</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="6" t="n">
         <v>1.0717</v>
       </c>
       <c r="K6" s="9" t="n">
         <v>0.0559</v>
       </c>
-      <c r="L6" s="5" t="n">
+      <c r="L6" s="6" t="n">
         <v>1.1548</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="6" t="n">
         <v>0.5446</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <v>0.0633</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="7" t="n">
         <v>0.1712</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <v>-1.9531</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="6" t="n">
         <v>-0.2151</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="7" t="n">
         <v>-1.463</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="7" t="n">
         <v>0.3025</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="6" t="n">
         <v>-2.2646</v>
       </c>
-      <c r="I7" s="5" t="n">
+      <c r="I7" s="6" t="n">
         <v>1.4417</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" s="6" t="n">
         <v>-1.2318</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="6" t="n">
         <v>-0.1403</v>
       </c>
-      <c r="L7" s="5" t="n">
+      <c r="L7" s="6" t="n">
         <v>-1.9814</v>
       </c>
-      <c r="M7" s="5" t="n">
+      <c r="M7" s="6" t="n">
         <v>-1.2117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="5" t="n">
         <v>-0.9169</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="5" t="n">
         <v>1.2958</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="5" t="n">
         <v>0.427</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="5" t="n">
         <v>-0.0712</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="5" t="n">
         <v>1.5911</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="5" t="n">
         <v>1.2566</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="5" t="n">
         <v>0.391</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="I8" s="5" t="n">
         <v>-0.3126</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="J8" s="5" t="n">
         <v>1.5823</v>
       </c>
-      <c r="K8" s="1" t="n">
+      <c r="K8" s="5" t="n">
         <v>2.7767</v>
       </c>
-      <c r="L8" s="1" t="n">
+      <c r="L8" s="5" t="n">
         <v>0.9466</v>
       </c>
-      <c r="M8" s="1" t="n">
+      <c r="M8" s="5" t="n">
         <v>1.4665</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="7" t="n">
         <v>-0.5489</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="6" t="n">
         <v>0.2491</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="6" t="n">
         <v>0.9036</v>
       </c>
-      <c r="F9" s="6" t="n">
+      <c r="F9" s="7" t="n">
         <v>-0.5302</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="7" t="n">
         <v>0.016</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="6" t="n">
         <v>-0.0997</v>
       </c>
-      <c r="I9" s="5" t="n">
+      <c r="I9" s="6" t="n">
         <v>1.0787</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="6" t="n">
         <v>-0.1371</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="6" t="n">
         <v>0.029</v>
       </c>
-      <c r="L9" s="5" t="n">
+      <c r="L9" s="6" t="n">
         <v>0.4011</v>
       </c>
-      <c r="M9" s="5" t="n">
+      <c r="M9" s="6" t="n">
         <v>0.0603</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="5" t="n">
         <v>1.0932</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="5" t="n">
         <v>0.4726</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="5" t="n">
         <v>1.1255</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="5" t="n">
         <v>0.6263</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="5" t="n">
         <v>0.5256</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="5" t="n">
         <v>-0.3325</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="5" t="n">
         <v>1.6525</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="I10" s="5" t="n">
         <v>-0.1135</v>
       </c>
-      <c r="J10" s="1" t="n">
+      <c r="J10" s="5" t="n">
         <v>0.61</v>
       </c>
-      <c r="K10" s="1" t="n">
+      <c r="K10" s="5" t="n">
         <v>0.6721</v>
       </c>
-      <c r="L10" s="1" t="n">
+      <c r="L10" s="5" t="n">
         <v>0.9582</v>
       </c>
-      <c r="M10" s="1" t="n">
+      <c r="M10" s="5" t="n">
         <v>0.3127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="5" t="n">
         <v>1.259</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="5" t="n">
         <v>1.0717</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="5" t="n">
         <v>0.916</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="5" t="n">
         <v>0.804</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="5" t="n">
         <v>-1.9025</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="5" t="n">
         <v>-0.4406</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="5" t="n">
         <v>0.5659</v>
       </c>
-      <c r="I11" s="1" t="n">
+      <c r="I11" s="5" t="n">
         <v>1.258</v>
       </c>
-      <c r="J11" s="1" t="n">
+      <c r="J11" s="5" t="n">
         <v>0.4927</v>
       </c>
-      <c r="K11" s="1" t="n">
+      <c r="K11" s="5" t="n">
         <v>0.2925</v>
       </c>
-      <c r="L11" s="1" t="n">
+      <c r="L11" s="5" t="n">
         <v>1.6588</v>
       </c>
-      <c r="M11" s="1" t="n">
+      <c r="M11" s="5" t="n">
         <v>1.1319</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="5" t="n">
         <v>-0.4763</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="5" t="n">
         <v>-0.4529</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="5" t="n">
         <v>-0.3336</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="5" t="n">
         <v>-0.5489</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="5" t="n">
         <v>2.5266</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="5" t="n">
         <v>0.4041</v>
       </c>
-      <c r="H12" s="1" t="n">
+      <c r="H12" s="5" t="n">
         <v>0.0257</v>
       </c>
-      <c r="I12" s="1" t="n">
+      <c r="I12" s="5" t="n">
         <v>-0.2142</v>
       </c>
-      <c r="J12" s="1" t="n">
+      <c r="J12" s="5" t="n">
         <v>-0.3101</v>
       </c>
-      <c r="K12" s="1" t="n">
+      <c r="K12" s="5" t="n">
         <v>0.905</v>
       </c>
-      <c r="L12" s="1" t="n">
+      <c r="L12" s="5" t="n">
         <v>0.092</v>
       </c>
-      <c r="M12" s="1" t="n">
+      <c r="M12" s="5" t="n">
         <v>0.2312</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="5" t="n">
         <v>-0.1331</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="5" t="n">
         <v>0.1802</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="5" t="n">
         <v>-0.3214</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="5" t="n">
         <v>-0.0182</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="5" t="n">
         <v>0.8526</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="5" t="n">
         <v>-0.4332</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="H13" s="5" t="n">
         <v>0.2249</v>
       </c>
-      <c r="I13" s="1" t="n">
+      <c r="I13" s="5" t="n">
         <v>-0.7035</v>
       </c>
-      <c r="J13" s="1" t="n">
+      <c r="J13" s="5" t="n">
         <v>0.0663</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="K13" s="5" t="n">
         <v>-0.4419</v>
       </c>
-      <c r="L13" s="1" t="n">
+      <c r="L13" s="5" t="n">
         <v>0.9222</v>
       </c>
-      <c r="M13" s="1" t="n">
+      <c r="M13" s="5" t="n">
         <v>0.209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="5" t="n">
         <v>-1.2421</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="5" t="n">
         <v>0.3344</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="5" t="n">
         <v>-0.735</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="5" t="n">
         <v>0.2935</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="5" t="n">
         <v>-1.2684</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="5" t="n">
         <v>-0.8782</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="5" t="n">
         <v>1.0021</v>
       </c>
-      <c r="I14" s="1" t="n">
+      <c r="I14" s="5" t="n">
         <v>-0.7668</v>
       </c>
-      <c r="J14" s="1" t="n">
+      <c r="J14" s="5" t="n">
         <v>0.9796</v>
       </c>
-      <c r="K14" s="1" t="n">
+      <c r="K14" s="5" t="n">
         <v>-0.0528</v>
       </c>
-      <c r="L14" s="1" t="n">
+      <c r="L14" s="5" t="n">
         <v>-0.8693</v>
       </c>
-      <c r="M14" s="1" t="n">
+      <c r="M14" s="5" t="n">
         <v>0.5579</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="5" t="n">
         <v>-1.3434</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="5" t="n">
         <v>-0.9354</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="5" t="n">
         <v>-1.7084</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="5" t="n">
         <v>-0.2822</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="5" t="n">
         <v>-0.0589</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="5" t="n">
         <v>-0.7158</v>
       </c>
-      <c r="H15" s="1" t="n">
+      <c r="H15" s="5" t="n">
         <v>-0.1155</v>
       </c>
-      <c r="I15" s="1" t="n">
+      <c r="I15" s="5" t="n">
         <v>-2.4802</v>
       </c>
-      <c r="J15" s="1" t="n">
+      <c r="J15" s="5" t="n">
         <v>0.6657</v>
       </c>
-      <c r="K15" s="1" t="n">
+      <c r="K15" s="5" t="n">
         <v>0.5316</v>
       </c>
-      <c r="L15" s="1" t="n">
+      <c r="L15" s="5" t="n">
         <v>-1.3987</v>
       </c>
-      <c r="M15" s="1" t="n">
+      <c r="M15" s="5" t="n">
         <v>0.2985</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="6" t="n">
         <v>0.8344</v>
       </c>
-      <c r="C16" s="6" t="n">
+      <c r="C16" s="7" t="n">
         <v>0.8398</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" s="6" t="n">
         <v>0.9184</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="6" t="n">
         <v>0.4747</v>
       </c>
-      <c r="F16" s="6" t="n">
+      <c r="F16" s="7" t="n">
         <v>2.3845</v>
       </c>
-      <c r="G16" s="6" t="n">
+      <c r="G16" s="7" t="n">
         <v>0.1525</v>
       </c>
-      <c r="H16" s="5" t="n">
+      <c r="H16" s="6" t="n">
         <v>0.6511</v>
       </c>
-      <c r="I16" s="5" t="n">
+      <c r="I16" s="6" t="n">
         <v>-0.8263</v>
       </c>
-      <c r="J16" s="5" t="n">
+      <c r="J16" s="6" t="n">
         <v>0.3113</v>
       </c>
-      <c r="K16" s="5" t="n">
+      <c r="K16" s="6" t="n">
         <v>-0.0906</v>
       </c>
-      <c r="L16" s="5" t="n">
+      <c r="L16" s="6" t="n">
         <v>0.9699</v>
       </c>
-      <c r="M16" s="5" t="n">
+      <c r="M16" s="6" t="n">
         <v>-0.0441</v>
       </c>
     </row>
@@ -3368,7 +3358,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3377,647 +3367,647 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="n">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="n">
+      <c r="D1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="n">
+      <c r="E1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G1" s="3" t="n">
+      <c r="G1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="H1" s="3" t="n">
+      <c r="H1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J1" s="3" t="n">
+      <c r="J1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="K1" s="3" t="n">
+      <c r="K1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="L1" s="3" t="n">
+      <c r="L1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="M1" s="3" t="n">
+      <c r="M1" s="4" t="n">
         <v>60</v>
       </c>
       <c r="N1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="5" t="n">
         <v>-0.8095</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="5" t="n">
         <v>-0.6243</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="5" t="n">
         <v>-1.1296</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="5" t="n">
         <v>-1.1113</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="5" t="n">
         <v>-1.408</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="5" t="n">
         <v>2.6021</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="5" t="n">
         <v>-0.4079</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="5" t="n">
         <v>1.2346</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="5" t="n">
         <v>1.1846</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="5" t="n">
         <v>-0.0588</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="L2" s="5" t="n">
         <v>0.4404</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="5" t="n">
         <v>-0.1933</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="5" t="n">
         <v>-1.0181</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="5" t="n">
         <v>-0.3813</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="5" t="n">
         <v>0.5164</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="5" t="n">
         <v>-0.17</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="5" t="n">
         <v>0.4056</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="5" t="n">
         <v>-0.3139</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="5" t="n">
         <v>-1.1147</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="5" t="n">
         <v>-0.9282</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="5" t="n">
         <v>0.9089</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="5" t="n">
         <v>-0.5136</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="L3" s="5" t="n">
         <v>-0.6743</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="M3" s="5" t="n">
         <v>-1.3101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="5" t="n">
         <v>1.452</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="5" t="n">
         <v>0.3668</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="5" t="n">
         <v>0.1465</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="5" t="n">
         <v>1.0023</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="5" t="n">
         <v>1.662</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="5" t="n">
         <v>2.9945</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="5" t="n">
         <v>1.3996</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="5" t="n">
         <v>1.9426</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="5" t="n">
         <v>0.2912</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="K4" s="5" t="n">
         <v>0.6282</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="L4" s="5" t="n">
         <v>3.2391</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="M4" s="5" t="n">
         <v>2.5788</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="5" t="n">
         <v>-0.5184</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="5" t="n">
         <v>1.3267</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="5" t="n">
         <v>1.0101</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="5" t="n">
         <v>-0.0616</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="1" t="n">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="n">
         <v>-0.1998</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="5" t="n">
         <v>1.1081</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="5" t="n">
         <v>0.1989</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="J5" s="5" t="n">
         <v>1.6447</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="K5" s="5" t="n">
         <v>-1.6054</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="L5" s="5" t="n">
         <v>0.7045</v>
       </c>
-      <c r="M5" s="1" t="n">
+      <c r="M5" s="5" t="n">
         <v>0.7673</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.5957</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="5" t="n">
         <v>0.8549</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="5" t="n">
         <v>-0.6759</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="5" t="n">
         <v>0.6343</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="5" t="n">
         <v>-0.0861</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="5" t="n">
         <v>-1.0684</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="5" t="n">
         <v>0.3023</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="5" t="n">
         <v>0.4177</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="J6" s="5" t="n">
         <v>0.1085</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="K6" s="5" t="n">
         <v>-0.446</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="L6" s="5" t="n">
         <v>0.8018</v>
       </c>
-      <c r="M6" s="1" t="n">
+      <c r="M6" s="5" t="n">
         <v>-0.161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="5" t="n">
         <v>3.3136</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="5" t="n">
         <v>1.8683</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="5" t="n">
         <v>0.9064</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="5" t="n">
         <v>0.2848</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="5" t="n">
         <v>1.2426</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="5" t="n">
         <v>1.4451</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="5" t="n">
         <v>0.9148</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="5" t="n">
         <v>-0.0132</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="J7" s="5" t="n">
         <v>1.2979</v>
       </c>
-      <c r="K7" s="1" t="n">
+      <c r="K7" s="5" t="n">
         <v>0.1059</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="L7" s="5" t="n">
         <v>-0.2976</v>
       </c>
-      <c r="M7" s="1" t="n">
+      <c r="M7" s="5" t="n">
         <v>0.2256</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.9772</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="5" t="n">
         <v>1.4618</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="5" t="n">
         <v>-0.7156</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="5" t="n">
         <v>0.7899</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="5" t="n">
         <v>1.5735</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="5" t="n">
         <v>1.1125</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="5" t="n">
         <v>1.1016</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="I8" s="5" t="n">
         <v>0.5146</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="J8" s="5" t="n">
         <v>1.3433</v>
       </c>
-      <c r="K8" s="1" t="n">
+      <c r="K8" s="5" t="n">
         <v>0.9501</v>
       </c>
-      <c r="L8" s="1" t="n">
+      <c r="L8" s="5" t="n">
         <v>1.5648</v>
       </c>
-      <c r="M8" s="1" t="n">
+      <c r="M8" s="5" t="n">
         <v>1.7134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="5" t="n">
         <v>1.0775</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="5" t="n">
         <v>-1.2575</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="5" t="n">
         <v>0.9656</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="5" t="n">
         <v>0.1669</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="5" t="n">
         <v>0.9394</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="5" t="n">
         <v>0.6417</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="5" t="n">
         <v>0.5814</v>
       </c>
-      <c r="I9" s="1" t="n">
+      <c r="I9" s="5" t="n">
         <v>2.5089</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="5" t="n">
         <v>0.8539</v>
       </c>
-      <c r="K9" s="1" t="n">
+      <c r="K9" s="5" t="n">
         <v>1.4608</v>
       </c>
-      <c r="L9" s="1" t="n">
+      <c r="L9" s="5" t="n">
         <v>0.7794</v>
       </c>
-      <c r="M9" s="1" t="n">
+      <c r="M9" s="5" t="n">
         <v>-0.287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="5" t="n">
         <v>-0.4157</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="5" t="n">
         <v>0.884</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="5" t="n">
         <v>1.2987</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="5" t="n">
         <v>1.3916</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="5" t="n">
         <v>1.055</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="5" t="n">
         <v>-0.6434</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="5" t="n">
         <v>2.4701</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="I10" s="5" t="n">
         <v>2.3169</v>
       </c>
-      <c r="J10" s="1" t="n">
+      <c r="J10" s="5" t="n">
         <v>1.2748</v>
       </c>
-      <c r="K10" s="1" t="n">
+      <c r="K10" s="5" t="n">
         <v>1.2483</v>
       </c>
-      <c r="L10" s="1" t="n">
+      <c r="L10" s="5" t="n">
         <v>0.2385</v>
       </c>
-      <c r="M10" s="1" t="n">
+      <c r="M10" s="5" t="n">
         <v>1.2221</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.8397</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="5" t="n">
         <v>0.8573</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="5" t="n">
         <v>0.2292</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="1" t="n">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="n">
         <v>1.1875</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="5" t="n">
         <v>0.2161</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="5" t="n">
         <v>0.0347</v>
       </c>
-      <c r="I11" s="1" t="n">
+      <c r="I11" s="5" t="n">
         <v>0.9642</v>
       </c>
-      <c r="J11" s="1" t="n">
+      <c r="J11" s="5" t="n">
         <v>0.7419</v>
       </c>
-      <c r="K11" s="1" t="n">
+      <c r="K11" s="5" t="n">
         <v>0.1088</v>
       </c>
-      <c r="L11" s="1" t="n">
+      <c r="L11" s="5" t="n">
         <v>0.6585</v>
       </c>
-      <c r="M11" s="1" t="n">
+      <c r="M11" s="5" t="n">
         <v>0.2671</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.1741</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="5" t="n">
         <v>-0.5323</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="5" t="n">
         <v>-1.2532</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="5" t="n">
         <v>-0.0805</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="5" t="n">
         <v>-0.3044</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="5" t="n">
         <v>0.44</v>
       </c>
-      <c r="H12" s="1" t="n">
+      <c r="H12" s="5" t="n">
         <v>-1.0187</v>
       </c>
-      <c r="I12" s="1" t="n">
+      <c r="I12" s="5" t="n">
         <v>-0.5621</v>
       </c>
-      <c r="J12" s="1" t="n">
+      <c r="J12" s="5" t="n">
         <v>-0.8838</v>
       </c>
-      <c r="K12" s="1" t="n">
+      <c r="K12" s="5" t="n">
         <v>0.9617</v>
       </c>
-      <c r="L12" s="1" t="n">
+      <c r="L12" s="5" t="n">
         <v>-0.8963</v>
       </c>
-      <c r="M12" s="1" t="n">
+      <c r="M12" s="5" t="n">
         <v>-0.2724</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="5" t="n">
         <v>-0.5215</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="5" t="n">
         <v>-1.3444</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="5" t="n">
         <v>0.4807</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="5" t="n">
         <v>0.0665</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="5" t="n">
         <v>-0.0551</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="5" t="n">
         <v>-0.2995</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="H13" s="5" t="n">
         <v>-0.4057</v>
       </c>
-      <c r="I13" s="1" t="n">
+      <c r="I13" s="5" t="n">
         <v>-0.4289</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="1" t="n">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5" t="n">
         <v>-0.9991</v>
       </c>
-      <c r="L13" s="1" t="n">
+      <c r="L13" s="5" t="n">
         <v>0.4751</v>
       </c>
-      <c r="M13" s="1" t="n">
+      <c r="M13" s="5" t="n">
         <v>0.2162</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="5" t="n">
         <v>-0.7022</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="5" t="n">
         <v>0.5408</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="5" t="n">
         <v>-0.0443</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="5" t="n">
         <v>0.5406</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="5" t="n">
         <v>0.8118</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="5" t="n">
         <v>0.9184</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="5" t="n">
         <v>2.4355</v>
       </c>
-      <c r="I14" s="1" t="n">
+      <c r="I14" s="5" t="n">
         <v>1.1496</v>
       </c>
-      <c r="J14" s="1" t="n">
+      <c r="J14" s="5" t="n">
         <v>1.0066</v>
       </c>
-      <c r="K14" s="1" t="n">
+      <c r="K14" s="5" t="n">
         <v>-0.2962</v>
       </c>
-      <c r="L14" s="1" t="n">
+      <c r="L14" s="5" t="n">
         <v>0.3564</v>
       </c>
-      <c r="M14" s="1" t="n">
+      <c r="M14" s="5" t="n">
         <v>1.0391</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="1" t="n">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="n">
         <v>0.5644</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="5" t="n">
         <v>-0.0194</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="5" t="n">
         <v>0.8211</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="5" t="n">
         <v>1.1649</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="5" t="n">
         <v>0.3713</v>
       </c>
-      <c r="H15" s="1" t="n">
+      <c r="H15" s="5" t="n">
         <v>0.6099</v>
       </c>
-      <c r="I15" s="1" t="n">
+      <c r="I15" s="5" t="n">
         <v>0.9206</v>
       </c>
-      <c r="J15" s="1" t="n">
+      <c r="J15" s="5" t="n">
         <v>0.9647</v>
       </c>
-      <c r="K15" s="1" t="n">
+      <c r="K15" s="5" t="n">
         <v>0.491</v>
       </c>
-      <c r="L15" s="1" t="n">
+      <c r="L15" s="5" t="n">
         <v>0.9253</v>
       </c>
-      <c r="M15" s="1" t="n">
+      <c r="M15" s="5" t="n">
         <v>1.2979</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="5" t="n">
         <v>-1.2207</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="5" t="n">
         <v>-0.2262</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="1" t="n">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="n">
         <v>0.405</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" s="5" t="n">
         <v>-0.5982</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G16" s="5" t="n">
         <v>1.7576</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="1" t="n">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5" t="n">
         <v>1.3799</v>
       </c>
-      <c r="J16" s="1" t="n">
+      <c r="J16" s="5" t="n">
         <v>-1.6436</v>
       </c>
-      <c r="K16" s="1" t="n">
+      <c r="K16" s="5" t="n">
         <v>-0.5111</v>
       </c>
-      <c r="L16" s="1" t="n">
+      <c r="L16" s="5" t="n">
         <v>-1.0852</v>
       </c>
-      <c r="M16" s="11"/>
+      <c r="M16" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4038,7 +4028,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4050,40 +4040,40 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="n">
+      <c r="B1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="n">
+      <c r="D1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="n">
+      <c r="E1" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G1" s="3" t="n">
+      <c r="G1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="H1" s="3" t="n">
+      <c r="H1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="J1" s="3" t="n">
+      <c r="J1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="K1" s="3" t="n">
+      <c r="K1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="L1" s="3" t="n">
+      <c r="L1" s="4" t="n">
         <v>60</v>
       </c>
-      <c r="M1" s="3" t="n">
+      <c r="M1" s="4" t="n">
         <v>60</v>
       </c>
       <c r="N1" s="3"/>
@@ -4092,40 +4082,40 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="5" t="n">
         <v>-0.558</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="5" t="n">
         <v>-0.313</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="5" t="n">
         <v>-0.0886</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="5" t="n">
         <v>0.5674</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="5" t="n">
         <v>-0.448</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="5" t="n">
         <v>-0.4768</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="5" t="n">
         <v>-0.598</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="5" t="n">
         <v>-0.1176</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="5" t="n">
         <v>-0.2783</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="5" t="n">
         <v>-0.6083</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="L2" s="5" t="n">
         <v>-0.6331</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="5" t="n">
         <v>0.1985</v>
       </c>
     </row>
@@ -4133,40 +4123,40 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="5" t="n">
         <v>-1.5401</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="5" t="n">
         <v>-0.0523</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="5" t="n">
         <v>-0.7026</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="5" t="n">
         <v>-0.4933</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="5" t="n">
         <v>-0.8167</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="5" t="n">
         <v>-0.0028</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="5" t="n">
         <v>-0.6568</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="5" t="n">
         <v>-1.0267</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="5" t="n">
         <v>-1.9867</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="5" t="n">
         <v>-1.5253</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="L3" s="5" t="n">
         <v>-1.0837</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="M3" s="5" t="n">
         <v>-1.5982</v>
       </c>
     </row>
@@ -4174,40 +4164,40 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="5" t="n">
         <v>-0.3943</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="5" t="n">
         <v>3.098</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="5" t="n">
         <v>-0.7818</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="5" t="n">
         <v>0.5366</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="5" t="n">
         <v>1.0477</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="5" t="n">
         <v>1.9388</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="5" t="n">
         <v>1.9985</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="5" t="n">
         <v>1.948</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="5" t="n">
         <v>2.8678</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="K4" s="5" t="n">
         <v>3.26</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="L4" s="5" t="n">
         <v>2.2513</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="M4" s="5" t="n">
         <v>1.9187</v>
       </c>
     </row>
@@ -4215,40 +4205,40 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="5" t="n">
         <v>1.5094</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="5" t="n">
         <v>0.4057</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="5" t="n">
         <v>0.5999</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="5" t="n">
         <v>1.291</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="5" t="n">
         <v>1.5787</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="5" t="n">
         <v>-0.5042</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="5" t="n">
         <v>1.659</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="5" t="n">
         <v>1.728</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="J5" s="5" t="n">
         <v>0.4889</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="K5" s="5" t="n">
         <v>-0.2991</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="L5" s="5" t="n">
         <v>0.9863</v>
       </c>
-      <c r="M5" s="1" t="n">
+      <c r="M5" s="5" t="n">
         <v>0.9578</v>
       </c>
     </row>
@@ -4256,40 +4246,40 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="5" t="n">
         <v>-0.4169</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="5" t="n">
         <v>0.6492</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="5" t="n">
         <v>-0.1259</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="5" t="n">
         <v>0.7149</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="5" t="n">
         <v>0.0457</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="5" t="n">
         <v>0.2932</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="5" t="n">
         <v>-0.3901</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="5" t="n">
         <v>0.2321</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="J6" s="5" t="n">
         <v>0.9238</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="K6" s="5" t="n">
         <v>0.3174</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="L6" s="5" t="n">
         <v>-0.0252</v>
       </c>
-      <c r="M6" s="1" t="n">
+      <c r="M6" s="5" t="n">
         <v>1.0246</v>
       </c>
     </row>
@@ -4297,40 +4287,40 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.4102</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="5" t="n">
         <v>-0.9203</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="5" t="n">
         <v>0.3786</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="5" t="n">
         <v>-0.8169</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="5" t="n">
         <v>0.0301</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="5" t="n">
         <v>-1.4462</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="5" t="n">
         <v>-0.3025</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="5" t="n">
         <v>-0.3727</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="J7" s="5" t="n">
         <v>-0.2195</v>
       </c>
-      <c r="K7" s="1" t="n">
+      <c r="K7" s="5" t="n">
         <v>-1.1639</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="L7" s="5" t="n">
         <v>0.2619</v>
       </c>
-      <c r="M7" s="1" t="n">
+      <c r="M7" s="5" t="n">
         <v>-0.5285</v>
       </c>
     </row>
@@ -4338,40 +4328,40 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="5" t="n">
         <v>2.9631</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="5" t="n">
         <v>0.0054</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="5" t="n">
         <v>1.0227</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="5" t="n">
         <v>-1.8079</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="5" t="n">
         <v>2.6496</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="5" t="n">
         <v>1.8897</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="5" t="n">
         <v>1.3275</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="I8" s="5" t="n">
         <v>-2.4363</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="J8" s="5" t="n">
         <v>1.3018</v>
       </c>
-      <c r="K8" s="1" t="n">
+      <c r="K8" s="5" t="n">
         <v>-0.2604</v>
       </c>
-      <c r="L8" s="1" t="n">
+      <c r="L8" s="5" t="n">
         <v>2.3205</v>
       </c>
-      <c r="M8" s="1" t="n">
+      <c r="M8" s="5" t="n">
         <v>-0.2676</v>
       </c>
     </row>
@@ -4379,40 +4369,40 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="5" t="n">
         <v>0.8346</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="5" t="n">
         <v>0.5458</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="5" t="n">
         <v>-0.4035</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="5" t="n">
         <v>0.5827</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="5" t="n">
         <v>1.0075</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="5" t="n">
         <v>0.8038</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="5" t="n">
         <v>1.1451</v>
       </c>
-      <c r="I9" s="1" t="n">
+      <c r="I9" s="5" t="n">
         <v>0.6532</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="5" t="n">
         <v>1.4213</v>
       </c>
-      <c r="K9" s="1" t="n">
+      <c r="K9" s="5" t="n">
         <v>0.7549</v>
       </c>
-      <c r="L9" s="1" t="n">
+      <c r="L9" s="5" t="n">
         <v>0.3324</v>
       </c>
-      <c r="M9" s="1" t="n">
+      <c r="M9" s="5" t="n">
         <v>0.3404</v>
       </c>
     </row>
@@ -4420,40 +4410,40 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.475</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="5" t="n">
         <v>0.8935</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="5" t="n">
         <v>0.0344</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="5" t="n">
         <v>0.9253</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="5" t="n">
         <v>-0.2822</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="5" t="n">
         <v>0.8125</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="5" t="n">
         <v>0.4466</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="I10" s="5" t="n">
         <v>0.3866</v>
       </c>
-      <c r="J10" s="1" t="n">
+      <c r="J10" s="5" t="n">
         <v>-0.1762</v>
       </c>
-      <c r="K10" s="1" t="n">
+      <c r="K10" s="5" t="n">
         <v>0.4906</v>
       </c>
-      <c r="L10" s="1" t="n">
+      <c r="L10" s="5" t="n">
         <v>0.4941</v>
       </c>
-      <c r="M10" s="1" t="n">
+      <c r="M10" s="5" t="n">
         <v>0.4523</v>
       </c>
     </row>
@@ -4461,34 +4451,34 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="5" t="n">
         <v>-0.1941</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="5" t="n">
         <v>-0.1977</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="5" t="n">
         <v>0.3222</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="1" t="n">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="n">
         <v>0.4058</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="5" t="n">
         <v>-0.84</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="5" t="n">
         <v>0.4143</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="1" t="n">
+      <c r="I11" s="5"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="5" t="n">
         <v>-0.1119</v>
       </c>
-      <c r="L11" s="1" t="n">
+      <c r="L11" s="5" t="n">
         <v>0.4121</v>
       </c>
-      <c r="M11" s="1" t="n">
+      <c r="M11" s="5" t="n">
         <v>0.1617</v>
       </c>
     </row>
@@ -4496,38 +4486,38 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="5" t="n">
         <v>0.857</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="5" t="n">
         <v>0.3944</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="5" t="n">
         <v>-0.0101</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="5" t="n">
         <v>-0.8563</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="5" t="n">
         <v>-0.1573</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="5" t="n">
         <v>-0.1339</v>
       </c>
-      <c r="H12" s="1" t="n">
+      <c r="H12" s="5" t="n">
         <v>-0.1171</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="1" t="n">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="n">
         <v>0.3775</v>
       </c>
-      <c r="K12" s="1" t="n">
+      <c r="K12" s="5" t="n">
         <v>0.4539</v>
       </c>
-      <c r="L12" s="1" t="n">
+      <c r="L12" s="5" t="n">
         <v>0.3331</v>
       </c>
-      <c r="M12" s="1" t="n">
+      <c r="M12" s="5" t="n">
         <v>0.2096</v>
       </c>
     </row>
@@ -4535,38 +4525,38 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="1" t="n">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="n">
         <v>0.1491</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="5" t="n">
         <v>-0.9615</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="5" t="n">
         <v>0.6945</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="5" t="n">
         <v>-1.177</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="5" t="n">
         <v>0.155</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="H13" s="5" t="n">
         <v>-1.3155</v>
       </c>
-      <c r="I13" s="1" t="n">
+      <c r="I13" s="5" t="n">
         <v>-0.1184</v>
       </c>
-      <c r="J13" s="1" t="n">
+      <c r="J13" s="5" t="n">
         <v>-1.0331</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="K13" s="5" t="n">
         <v>0.07</v>
       </c>
-      <c r="L13" s="1" t="n">
+      <c r="L13" s="5" t="n">
         <v>-0.7403</v>
       </c>
-      <c r="M13" s="1" t="n">
+      <c r="M13" s="5" t="n">
         <v>0.728</v>
       </c>
     </row>
@@ -4574,40 +4564,40 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="5" t="n">
         <v>-0.8778</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="5" t="n">
         <v>-0.5421</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="5" t="n">
         <v>-1.4449</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="5" t="n">
         <v>-0.6419</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="5" t="n">
         <v>-0.986</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="5" t="n">
         <v>-0.0224</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="5" t="n">
         <v>-0.4459</v>
       </c>
-      <c r="I14" s="1" t="n">
+      <c r="I14" s="5" t="n">
         <v>-0.1383</v>
       </c>
-      <c r="J14" s="1" t="n">
+      <c r="J14" s="5" t="n">
         <v>0.9324</v>
       </c>
-      <c r="K14" s="1" t="n">
+      <c r="K14" s="5" t="n">
         <v>1.2889</v>
       </c>
-      <c r="L14" s="1" t="n">
+      <c r="L14" s="5" t="n">
         <v>0.6571</v>
       </c>
-      <c r="M14" s="1" t="n">
+      <c r="M14" s="5" t="n">
         <v>0.9774</v>
       </c>
     </row>
@@ -4615,40 +4605,40 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="5" t="n">
         <v>-1.7099</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="5" t="n">
         <v>-1.3898</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="D15" s="5" t="n">
         <v>-2.1356</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="5" t="n">
         <v>-1.6842</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="5" t="n">
         <v>-0.1238</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="5" t="n">
         <v>-1.0174</v>
       </c>
-      <c r="H15" s="1" t="n">
+      <c r="H15" s="5" t="n">
         <v>0.37</v>
       </c>
-      <c r="I15" s="1" t="n">
+      <c r="I15" s="5" t="n">
         <v>-1.6723</v>
       </c>
-      <c r="J15" s="1" t="n">
+      <c r="J15" s="5" t="n">
         <v>-0.259</v>
       </c>
-      <c r="K15" s="1" t="n">
+      <c r="K15" s="5" t="n">
         <v>-0.2008</v>
       </c>
-      <c r="L15" s="1" t="n">
+      <c r="L15" s="5" t="n">
         <v>-1.5284</v>
       </c>
-      <c r="M15" s="1" t="n">
+      <c r="M15" s="5" t="n">
         <v>-1.0413</v>
       </c>
     </row>
@@ -4656,38 +4646,38 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="5" t="n">
         <v>-1.903</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="1" t="n">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="n">
         <v>1.5545</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="5" t="n">
         <v>-0.0849</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" s="5" t="n">
         <v>-0.6127</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G16" s="5" t="n">
         <v>1.2343</v>
       </c>
-      <c r="H16" s="1" t="n">
+      <c r="H16" s="5" t="n">
         <v>-0.5888</v>
       </c>
-      <c r="I16" s="1" t="n">
+      <c r="I16" s="5" t="n">
         <v>-0.8746</v>
       </c>
-      <c r="J16" s="1" t="n">
+      <c r="J16" s="5" t="n">
         <v>-0.8822</v>
       </c>
-      <c r="K16" s="1" t="n">
+      <c r="K16" s="5" t="n">
         <v>0.6754</v>
       </c>
-      <c r="L16" s="1" t="n">
+      <c r="L16" s="5" t="n">
         <v>-0.7341</v>
       </c>
-      <c r="M16" s="1" t="n">
+      <c r="M16" s="5" t="n">
         <v>-0.5958</v>
       </c>
     </row>
@@ -4709,8 +4699,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5139,26 +5129,26 @@
       <c r="C11" s="1" t="n">
         <v>0.5574</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="1" t="n">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="n">
         <v>0.297</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="5" t="n">
         <v>0.1843</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="5" t="n">
         <v>0.1582</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="1" t="n">
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="n">
         <v>1.7097</v>
       </c>
-      <c r="K11" s="1" t="n">
+      <c r="K11" s="5" t="n">
         <v>0.6198</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -5383,8 +5373,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5520,7 +5510,7 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="n">
         <v>2.4162</v>
       </c>
@@ -5559,7 +5549,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="5" t="n">
         <v>0.6693</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -5600,7 +5590,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="5" t="n">
         <v>0.4944</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -5641,7 +5631,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="5" t="n">
         <v>0.9889</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -5682,7 +5672,7 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="5" t="n">
         <v>0.3519</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -5723,7 +5713,7 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="5" t="n">
         <v>-0.1455</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -5764,7 +5754,7 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="5" t="n">
         <v>0.5518</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -5791,7 +5781,7 @@
       <c r="J10" s="1" t="n">
         <v>-0.6863</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="K10" s="12" t="n">
         <v>0.0001</v>
       </c>
       <c r="L10" s="1" t="n">
@@ -5805,7 +5795,7 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="5" t="n">
         <v>0.3316</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -5846,7 +5836,7 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="5" t="n">
         <v>-0.0389</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -5887,7 +5877,7 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="5" t="n">
         <v>-1.0275</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -5928,7 +5918,7 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="5" t="n">
         <v>-0.7061</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -5969,7 +5959,7 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="5" t="n">
         <v>-1.7194</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -6010,7 +6000,7 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="1" t="n">
         <v>0.1287</v>
       </c>
@@ -6032,7 +6022,7 @@
       <c r="I16" s="1" t="n">
         <v>-0.2373</v>
       </c>
-      <c r="J16" s="11"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="1" t="n">
         <v>0.6914</v>
       </c>
@@ -6061,8 +6051,8 @@
   </sheetPr>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
altered test files to include workbook type, in order to pass tests
</commit_message>
<xml_diff>
--- a/test-files/additional-sheet-test-files/optimization-parameters-default.xlsx
+++ b/test-files/additional-sheet-test-files/optimization-parameters-default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="49">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -171,6 +171,12 @@
     <t xml:space="preserve">taxon_id</t>
   </si>
   <si>
+    <t xml:space="preserve">workbookType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grn</t>
+  </si>
+  <si>
     <t xml:space="preserve">threshold_b</t>
   </si>
 </sst>
@@ -295,7 +301,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -309,14 +315,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,23 +338,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -422,7 +416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -432,11 +426,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -569,8 +563,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -579,7 +573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -589,9 +583,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,8 +1390,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1406,21 +1400,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,7 +1429,7 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="12" t="n">
+      <c r="B2" s="9" t="n">
         <v>0.002</v>
       </c>
     </row>
@@ -1451,7 +1445,7 @@
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="9" t="n">
         <v>100000000</v>
       </c>
     </row>
@@ -1459,7 +1453,7 @@
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="9" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -1467,7 +1461,7 @@
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="12" t="n">
+      <c r="B6" s="9" t="n">
         <v>100000000</v>
       </c>
     </row>
@@ -1475,7 +1469,7 @@
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="12" t="n">
+      <c r="B7" s="9" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -1624,10 +1618,18 @@
         <v>559292</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1636,19 +1638,19 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,8 +1783,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1791,7 +1793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1801,11 +1803,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,8 +1940,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1948,7 +1950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1958,9 +1960,9 @@
       <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,7 +2028,7 @@
       <c r="F2" s="3" t="n">
         <v>0.5827</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="3" t="n">
         <v>-0.3947</v>
       </c>
@@ -2661,12 +2663,12 @@
       <c r="M16" s="3" t="n">
         <v>1.3863</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="N16" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2675,7 +2677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2685,664 +2687,664 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="5" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="n">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="n">
+      <c r="C1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="D1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="n">
+      <c r="E1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="n">
+      <c r="F1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="G1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="n">
+      <c r="H1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I1" s="4" t="n">
+      <c r="I1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="K1" s="4" t="n">
+      <c r="K1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="L1" s="4" t="n">
+      <c r="L1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="M1" s="4" t="n">
+      <c r="M1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="N1" s="4"/>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="4" t="n">
         <v>-0.1718</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="5" t="n">
         <v>-0.2792</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="4" t="n">
         <v>-0.1752</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="4" t="n">
         <v>-0.6884</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="5" t="n">
         <v>-0.2436</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="5" t="n">
         <v>0.1581</v>
       </c>
-      <c r="H2" s="6" t="n">
+      <c r="H2" s="4" t="n">
         <v>-0.4253</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="6" t="n">
+      <c r="I2" s="6"/>
+      <c r="J2" s="4" t="n">
         <v>0.5682</v>
       </c>
-      <c r="K2" s="6" t="n">
+      <c r="K2" s="4" t="n">
         <v>0.1646</v>
       </c>
-      <c r="L2" s="6" t="n">
+      <c r="L2" s="4" t="n">
         <v>-0.3202</v>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="M2" s="4" t="n">
         <v>-0.3888</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="1" t="n">
         <v>-1.3229</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="1" t="n">
         <v>-0.4236</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="1" t="n">
         <v>-1.8945</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="1" t="n">
         <v>-1.6929</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="1" t="n">
         <v>-2.2704</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="1" t="n">
         <v>-1.0939</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="1" t="n">
         <v>-1.3098</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="1" t="n">
         <v>-1.017</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" s="1" t="n">
         <v>-1.7106</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="1" t="n">
         <v>-1.7777</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="1" t="n">
         <v>-1.9029</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="1" t="n">
         <v>-1.3284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="4" t="n">
         <v>-0.6685</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6" t="n">
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="n">
         <v>-0.4322</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="4" t="n">
         <v>-0.1191</v>
       </c>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="5" t="n">
         <v>-0.383</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="G4" s="5" t="n">
         <v>0.2693</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="4" t="n">
         <v>-0.0757</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="4" t="n">
         <v>0.5975</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="6" t="n">
+      <c r="J4" s="6"/>
+      <c r="K4" s="4" t="n">
         <v>-0.3216</v>
       </c>
-      <c r="L4" s="6" t="n">
+      <c r="L4" s="4" t="n">
         <v>0.0805</v>
       </c>
-      <c r="M4" s="6" t="n">
+      <c r="M4" s="4" t="n">
         <v>0.4778</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="4" t="n">
         <v>-0.3155</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="5" t="n">
         <v>1.4649</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="4" t="n">
         <v>-0.8029</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="4" t="n">
         <v>0.5141</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="5" t="n">
         <v>-0.7654</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="5" t="n">
         <v>-1.1456</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="4" t="n">
         <v>0.5096</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="4" t="n">
         <v>-0.2957</v>
       </c>
-      <c r="J5" s="6" t="n">
+      <c r="J5" s="4" t="n">
         <v>-0.2257</v>
       </c>
-      <c r="K5" s="6" t="n">
+      <c r="K5" s="4" t="n">
         <v>-0.9404</v>
       </c>
-      <c r="L5" s="6" t="n">
+      <c r="L5" s="4" t="n">
         <v>-1.3326</v>
       </c>
-      <c r="M5" s="6" t="n">
+      <c r="M5" s="4" t="n">
         <v>0.1689</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="4" t="n">
         <v>0.9621</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="5" t="n">
         <v>-0.3518</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="4" t="n">
         <v>0.3101</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="4" t="n">
         <v>-0.1589</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="5" t="n">
         <v>0.5869</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="5" t="n">
         <v>0.0341</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="4" t="n">
         <v>0.486</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="4" t="n">
         <v>0.4342</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J6" s="4" t="n">
         <v>1.0717</v>
       </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="7" t="n">
         <v>0.0559</v>
       </c>
-      <c r="L6" s="6" t="n">
+      <c r="L6" s="4" t="n">
         <v>1.1548</v>
       </c>
-      <c r="M6" s="6" t="n">
+      <c r="M6" s="4" t="n">
         <v>0.5446</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="4" t="n">
         <v>0.0633</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="5" t="n">
         <v>0.1712</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="4" t="n">
         <v>-1.9531</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="4" t="n">
         <v>-0.2151</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="5" t="n">
         <v>-1.463</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="5" t="n">
         <v>0.3025</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="H7" s="4" t="n">
         <v>-2.2646</v>
       </c>
-      <c r="I7" s="6" t="n">
+      <c r="I7" s="4" t="n">
         <v>1.4417</v>
       </c>
-      <c r="J7" s="6" t="n">
+      <c r="J7" s="4" t="n">
         <v>-1.2318</v>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="K7" s="4" t="n">
         <v>-0.1403</v>
       </c>
-      <c r="L7" s="6" t="n">
+      <c r="L7" s="4" t="n">
         <v>-1.9814</v>
       </c>
-      <c r="M7" s="6" t="n">
+      <c r="M7" s="4" t="n">
         <v>-1.2117</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="1" t="n">
         <v>-0.9169</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="1" t="n">
         <v>1.2958</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="1" t="n">
         <v>0.427</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="1" t="n">
         <v>-0.0712</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="1" t="n">
         <v>1.5911</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="1" t="n">
         <v>1.2566</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="1" t="n">
         <v>0.391</v>
       </c>
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="1" t="n">
         <v>-0.3126</v>
       </c>
-      <c r="J8" s="5" t="n">
+      <c r="J8" s="1" t="n">
         <v>1.5823</v>
       </c>
-      <c r="K8" s="5" t="n">
+      <c r="K8" s="1" t="n">
         <v>2.7767</v>
       </c>
-      <c r="L8" s="5" t="n">
+      <c r="L8" s="1" t="n">
         <v>0.9466</v>
       </c>
-      <c r="M8" s="5" t="n">
+      <c r="M8" s="1" t="n">
         <v>1.4665</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="7" t="n">
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="n">
         <v>-0.5489</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="4" t="n">
         <v>0.2491</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="4" t="n">
         <v>0.9036</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="5" t="n">
         <v>-0.5302</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="5" t="n">
         <v>0.016</v>
       </c>
-      <c r="H9" s="6" t="n">
+      <c r="H9" s="4" t="n">
         <v>-0.0997</v>
       </c>
-      <c r="I9" s="6" t="n">
+      <c r="I9" s="4" t="n">
         <v>1.0787</v>
       </c>
-      <c r="J9" s="6" t="n">
+      <c r="J9" s="4" t="n">
         <v>-0.1371</v>
       </c>
-      <c r="K9" s="6" t="n">
+      <c r="K9" s="4" t="n">
         <v>0.029</v>
       </c>
-      <c r="L9" s="6" t="n">
+      <c r="L9" s="4" t="n">
         <v>0.4011</v>
       </c>
-      <c r="M9" s="6" t="n">
+      <c r="M9" s="4" t="n">
         <v>0.0603</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="1" t="n">
         <v>1.0932</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.4726</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="1" t="n">
         <v>1.1255</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="1" t="n">
         <v>0.6263</v>
       </c>
-      <c r="F10" s="5" t="n">
+      <c r="F10" s="1" t="n">
         <v>0.5256</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="1" t="n">
         <v>-0.3325</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="1" t="n">
         <v>1.6525</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="1" t="n">
         <v>-0.1135</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" s="1" t="n">
         <v>0.61</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="1" t="n">
         <v>0.6721</v>
       </c>
-      <c r="L10" s="5" t="n">
+      <c r="L10" s="1" t="n">
         <v>0.9582</v>
       </c>
-      <c r="M10" s="5" t="n">
+      <c r="M10" s="1" t="n">
         <v>0.3127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="1" t="n">
         <v>1.259</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="1" t="n">
         <v>1.0717</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="1" t="n">
         <v>0.916</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="1" t="n">
         <v>0.804</v>
       </c>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="1" t="n">
         <v>-1.9025</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="1" t="n">
         <v>-0.4406</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="1" t="n">
         <v>0.5659</v>
       </c>
-      <c r="I11" s="5" t="n">
+      <c r="I11" s="1" t="n">
         <v>1.258</v>
       </c>
-      <c r="J11" s="5" t="n">
+      <c r="J11" s="1" t="n">
         <v>0.4927</v>
       </c>
-      <c r="K11" s="5" t="n">
+      <c r="K11" s="1" t="n">
         <v>0.2925</v>
       </c>
-      <c r="L11" s="5" t="n">
+      <c r="L11" s="1" t="n">
         <v>1.6588</v>
       </c>
-      <c r="M11" s="5" t="n">
+      <c r="M11" s="1" t="n">
         <v>1.1319</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="1" t="n">
         <v>-0.4763</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="1" t="n">
         <v>-0.4529</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="1" t="n">
         <v>-0.3336</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="1" t="n">
         <v>-0.5489</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="1" t="n">
         <v>2.5266</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="1" t="n">
         <v>0.4041</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="1" t="n">
         <v>0.0257</v>
       </c>
-      <c r="I12" s="5" t="n">
+      <c r="I12" s="1" t="n">
         <v>-0.2142</v>
       </c>
-      <c r="J12" s="5" t="n">
+      <c r="J12" s="1" t="n">
         <v>-0.3101</v>
       </c>
-      <c r="K12" s="5" t="n">
+      <c r="K12" s="1" t="n">
         <v>0.905</v>
       </c>
-      <c r="L12" s="5" t="n">
+      <c r="L12" s="1" t="n">
         <v>0.092</v>
       </c>
-      <c r="M12" s="5" t="n">
+      <c r="M12" s="1" t="n">
         <v>0.2312</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="1" t="n">
         <v>-0.1331</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.1802</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="1" t="n">
         <v>-0.3214</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="1" t="n">
         <v>-0.0182</v>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="1" t="n">
         <v>0.8526</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="1" t="n">
         <v>-0.4332</v>
       </c>
-      <c r="H13" s="5" t="n">
+      <c r="H13" s="1" t="n">
         <v>0.2249</v>
       </c>
-      <c r="I13" s="5" t="n">
+      <c r="I13" s="1" t="n">
         <v>-0.7035</v>
       </c>
-      <c r="J13" s="5" t="n">
+      <c r="J13" s="1" t="n">
         <v>0.0663</v>
       </c>
-      <c r="K13" s="5" t="n">
+      <c r="K13" s="1" t="n">
         <v>-0.4419</v>
       </c>
-      <c r="L13" s="5" t="n">
+      <c r="L13" s="1" t="n">
         <v>0.9222</v>
       </c>
-      <c r="M13" s="5" t="n">
+      <c r="M13" s="1" t="n">
         <v>0.209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="1" t="n">
         <v>-1.2421</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.3344</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="1" t="n">
         <v>-0.735</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="1" t="n">
         <v>0.2935</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="1" t="n">
         <v>-1.2684</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="1" t="n">
         <v>-0.8782</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="1" t="n">
         <v>1.0021</v>
       </c>
-      <c r="I14" s="5" t="n">
+      <c r="I14" s="1" t="n">
         <v>-0.7668</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" s="1" t="n">
         <v>0.9796</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="1" t="n">
         <v>-0.0528</v>
       </c>
-      <c r="L14" s="5" t="n">
+      <c r="L14" s="1" t="n">
         <v>-0.8693</v>
       </c>
-      <c r="M14" s="5" t="n">
+      <c r="M14" s="1" t="n">
         <v>0.5579</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="1" t="n">
         <v>-1.3434</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="1" t="n">
         <v>-0.9354</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="1" t="n">
         <v>-1.7084</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="1" t="n">
         <v>-0.2822</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="1" t="n">
         <v>-0.0589</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="1" t="n">
         <v>-0.7158</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="1" t="n">
         <v>-0.1155</v>
       </c>
-      <c r="I15" s="5" t="n">
+      <c r="I15" s="1" t="n">
         <v>-2.4802</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" s="1" t="n">
         <v>0.6657</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="1" t="n">
         <v>0.5316</v>
       </c>
-      <c r="L15" s="5" t="n">
+      <c r="L15" s="1" t="n">
         <v>-1.3987</v>
       </c>
-      <c r="M15" s="5" t="n">
+      <c r="M15" s="1" t="n">
         <v>0.2985</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="4" t="n">
         <v>0.8344</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="5" t="n">
         <v>0.8398</v>
       </c>
-      <c r="D16" s="6" t="n">
+      <c r="D16" s="4" t="n">
         <v>0.9184</v>
       </c>
-      <c r="E16" s="6" t="n">
+      <c r="E16" s="4" t="n">
         <v>0.4747</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="5" t="n">
         <v>2.3845</v>
       </c>
-      <c r="G16" s="7" t="n">
+      <c r="G16" s="5" t="n">
         <v>0.1525</v>
       </c>
-      <c r="H16" s="6" t="n">
+      <c r="H16" s="4" t="n">
         <v>0.6511</v>
       </c>
-      <c r="I16" s="6" t="n">
+      <c r="I16" s="4" t="n">
         <v>-0.8263</v>
       </c>
-      <c r="J16" s="6" t="n">
+      <c r="J16" s="4" t="n">
         <v>0.3113</v>
       </c>
-      <c r="K16" s="6" t="n">
+      <c r="K16" s="4" t="n">
         <v>-0.0906</v>
       </c>
-      <c r="L16" s="6" t="n">
+      <c r="L16" s="4" t="n">
         <v>0.9699</v>
       </c>
-      <c r="M16" s="6" t="n">
+      <c r="M16" s="4" t="n">
         <v>-0.0441</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3351,7 +3353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3361,658 +3363,651 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="n">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="n">
+      <c r="C1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="D1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="n">
+      <c r="E1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="n">
+      <c r="F1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="G1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="n">
+      <c r="H1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I1" s="4" t="n">
+      <c r="I1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="K1" s="4" t="n">
+      <c r="K1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="L1" s="4" t="n">
+      <c r="L1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="M1" s="4" t="n">
+      <c r="M1" s="3" t="n">
         <v>60</v>
       </c>
       <c r="N1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="1" t="n">
         <v>-0.8095</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="1" t="n">
         <v>-0.6243</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="1" t="n">
         <v>-1.1296</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="1" t="n">
         <v>-1.1113</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="1" t="n">
         <v>-1.408</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="1" t="n">
         <v>2.6021</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="1" t="n">
         <v>-0.4079</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="1" t="n">
         <v>1.2346</v>
       </c>
-      <c r="J2" s="5" t="n">
+      <c r="J2" s="1" t="n">
         <v>1.1846</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="K2" s="1" t="n">
         <v>-0.0588</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="1" t="n">
         <v>0.4404</v>
       </c>
-      <c r="M2" s="5" t="n">
+      <c r="M2" s="1" t="n">
         <v>-0.1933</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="1" t="n">
         <v>-1.0181</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="1" t="n">
         <v>-0.3813</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.5164</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="1" t="n">
         <v>-0.17</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.4056</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="1" t="n">
         <v>-0.3139</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="1" t="n">
         <v>-1.1147</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="1" t="n">
         <v>-0.9282</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" s="1" t="n">
         <v>0.9089</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="1" t="n">
         <v>-0.5136</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="1" t="n">
         <v>-0.6743</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="1" t="n">
         <v>-1.3101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="1" t="n">
         <v>1.452</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.3668</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.1465</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="1" t="n">
         <v>1.0023</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="1" t="n">
         <v>1.662</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="1" t="n">
         <v>2.9945</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="1" t="n">
         <v>1.3996</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="1" t="n">
         <v>1.9426</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.2912</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="1" t="n">
         <v>0.6282</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="1" t="n">
         <v>3.2391</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="1" t="n">
         <v>2.5788</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="1" t="n">
         <v>-0.5184</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="1" t="n">
         <v>1.3267</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="1" t="n">
         <v>1.0101</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="1" t="n">
         <v>-0.0616</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="1" t="n">
         <v>-0.1998</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="1" t="n">
         <v>1.1081</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="1" t="n">
         <v>0.1989</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="1" t="n">
         <v>1.6447</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="1" t="n">
         <v>-1.6054</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="1" t="n">
         <v>0.7045</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="1" t="n">
         <v>0.7673</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="1" t="n">
         <v>0.5957</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.8549</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="1" t="n">
         <v>-0.6759</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="1" t="n">
         <v>0.6343</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="1" t="n">
         <v>-0.0861</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="1" t="n">
         <v>-1.0684</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="1" t="n">
         <v>0.3023</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="1" t="n">
         <v>0.4177</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="1" t="n">
         <v>0.1085</v>
       </c>
-      <c r="K6" s="5" t="n">
+      <c r="K6" s="1" t="n">
         <v>-0.446</v>
       </c>
-      <c r="L6" s="5" t="n">
+      <c r="L6" s="1" t="n">
         <v>0.8018</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="1" t="n">
         <v>-0.161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="1" t="n">
         <v>3.3136</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="1" t="n">
         <v>1.8683</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="1" t="n">
         <v>0.9064</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="1" t="n">
         <v>0.2848</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="1" t="n">
         <v>1.2426</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="1" t="n">
         <v>1.4451</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="1" t="n">
         <v>0.9148</v>
       </c>
-      <c r="I7" s="5" t="n">
+      <c r="I7" s="1" t="n">
         <v>-0.0132</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" s="1" t="n">
         <v>1.2979</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="1" t="n">
         <v>0.1059</v>
       </c>
-      <c r="L7" s="5" t="n">
+      <c r="L7" s="1" t="n">
         <v>-0.2976</v>
       </c>
-      <c r="M7" s="5" t="n">
+      <c r="M7" s="1" t="n">
         <v>0.2256</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="1" t="n">
         <v>0.9772</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="1" t="n">
         <v>1.4618</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="1" t="n">
         <v>-0.7156</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="1" t="n">
         <v>0.7899</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="1" t="n">
         <v>1.5735</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="1" t="n">
         <v>1.1125</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="1" t="n">
         <v>1.1016</v>
       </c>
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="1" t="n">
         <v>0.5146</v>
       </c>
-      <c r="J8" s="5" t="n">
+      <c r="J8" s="1" t="n">
         <v>1.3433</v>
       </c>
-      <c r="K8" s="5" t="n">
+      <c r="K8" s="1" t="n">
         <v>0.9501</v>
       </c>
-      <c r="L8" s="5" t="n">
+      <c r="L8" s="1" t="n">
         <v>1.5648</v>
       </c>
-      <c r="M8" s="5" t="n">
+      <c r="M8" s="1" t="n">
         <v>1.7134</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="1" t="n">
         <v>1.0775</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="1" t="n">
         <v>-1.2575</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="1" t="n">
         <v>0.9656</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="1" t="n">
         <v>0.1669</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="1" t="n">
         <v>0.9394</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.6417</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="1" t="n">
         <v>0.5814</v>
       </c>
-      <c r="I9" s="5" t="n">
+      <c r="I9" s="1" t="n">
         <v>2.5089</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="1" t="n">
         <v>0.8539</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="1" t="n">
         <v>1.4608</v>
       </c>
-      <c r="L9" s="5" t="n">
+      <c r="L9" s="1" t="n">
         <v>0.7794</v>
       </c>
-      <c r="M9" s="5" t="n">
+      <c r="M9" s="1" t="n">
         <v>-0.287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="1" t="n">
         <v>-0.4157</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.884</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="1" t="n">
         <v>1.2987</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="1" t="n">
         <v>1.3916</v>
       </c>
-      <c r="F10" s="5" t="n">
+      <c r="F10" s="1" t="n">
         <v>1.055</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="1" t="n">
         <v>-0.6434</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="1" t="n">
         <v>2.4701</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="1" t="n">
         <v>2.3169</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" s="1" t="n">
         <v>1.2748</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="1" t="n">
         <v>1.2483</v>
       </c>
-      <c r="L10" s="5" t="n">
+      <c r="L10" s="1" t="n">
         <v>0.2385</v>
       </c>
-      <c r="M10" s="5" t="n">
+      <c r="M10" s="1" t="n">
         <v>1.2221</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="1" t="n">
         <v>0.8397</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="1" t="n">
         <v>0.8573</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="1" t="n">
         <v>0.2292</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="1" t="n">
         <v>1.1875</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="1" t="n">
         <v>0.2161</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="1" t="n">
         <v>0.0347</v>
       </c>
-      <c r="I11" s="5" t="n">
+      <c r="I11" s="1" t="n">
         <v>0.9642</v>
       </c>
-      <c r="J11" s="5" t="n">
+      <c r="J11" s="1" t="n">
         <v>0.7419</v>
       </c>
-      <c r="K11" s="5" t="n">
+      <c r="K11" s="1" t="n">
         <v>0.1088</v>
       </c>
-      <c r="L11" s="5" t="n">
+      <c r="L11" s="1" t="n">
         <v>0.6585</v>
       </c>
-      <c r="M11" s="5" t="n">
+      <c r="M11" s="1" t="n">
         <v>0.2671</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="1" t="n">
         <v>0.1741</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="1" t="n">
         <v>-0.5323</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="1" t="n">
         <v>-1.2532</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="1" t="n">
         <v>-0.0805</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="1" t="n">
         <v>-0.3044</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="1" t="n">
         <v>0.44</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="1" t="n">
         <v>-1.0187</v>
       </c>
-      <c r="I12" s="5" t="n">
+      <c r="I12" s="1" t="n">
         <v>-0.5621</v>
       </c>
-      <c r="J12" s="5" t="n">
+      <c r="J12" s="1" t="n">
         <v>-0.8838</v>
       </c>
-      <c r="K12" s="5" t="n">
+      <c r="K12" s="1" t="n">
         <v>0.9617</v>
       </c>
-      <c r="L12" s="5" t="n">
+      <c r="L12" s="1" t="n">
         <v>-0.8963</v>
       </c>
-      <c r="M12" s="5" t="n">
+      <c r="M12" s="1" t="n">
         <v>-0.2724</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="1" t="n">
         <v>-0.5215</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="1" t="n">
         <v>-1.3444</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="1" t="n">
         <v>0.4807</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="1" t="n">
         <v>0.0665</v>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="1" t="n">
         <v>-0.0551</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="1" t="n">
         <v>-0.2995</v>
       </c>
-      <c r="H13" s="5" t="n">
+      <c r="H13" s="1" t="n">
         <v>-0.4057</v>
       </c>
-      <c r="I13" s="5" t="n">
+      <c r="I13" s="1" t="n">
         <v>-0.4289</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5" t="n">
+      <c r="K13" s="1" t="n">
         <v>-0.9991</v>
       </c>
-      <c r="L13" s="5" t="n">
+      <c r="L13" s="1" t="n">
         <v>0.4751</v>
       </c>
-      <c r="M13" s="5" t="n">
+      <c r="M13" s="1" t="n">
         <v>0.2162</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="1" t="n">
         <v>-0.7022</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.5408</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="1" t="n">
         <v>-0.0443</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="1" t="n">
         <v>0.5406</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="1" t="n">
         <v>0.8118</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="1" t="n">
         <v>0.9184</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="1" t="n">
         <v>2.4355</v>
       </c>
-      <c r="I14" s="5" t="n">
+      <c r="I14" s="1" t="n">
         <v>1.1496</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" s="1" t="n">
         <v>1.0066</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="1" t="n">
         <v>-0.2962</v>
       </c>
-      <c r="L14" s="5" t="n">
+      <c r="L14" s="1" t="n">
         <v>0.3564</v>
       </c>
-      <c r="M14" s="5" t="n">
+      <c r="M14" s="1" t="n">
         <v>1.0391</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.5644</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="1" t="n">
         <v>-0.0194</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="1" t="n">
         <v>0.8211</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="1" t="n">
         <v>1.1649</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="1" t="n">
         <v>0.3713</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="1" t="n">
         <v>0.6099</v>
       </c>
-      <c r="I15" s="5" t="n">
+      <c r="I15" s="1" t="n">
         <v>0.9206</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" s="1" t="n">
         <v>0.9647</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="1" t="n">
         <v>0.491</v>
       </c>
-      <c r="L15" s="5" t="n">
+      <c r="L15" s="1" t="n">
         <v>0.9253</v>
       </c>
-      <c r="M15" s="5" t="n">
+      <c r="M15" s="1" t="n">
         <v>1.2979</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="1" t="n">
         <v>-1.2207</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="1" t="n">
         <v>-0.2262</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="1" t="n">
         <v>0.405</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="1" t="n">
         <v>-0.5982</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="1" t="n">
         <v>1.7576</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5" t="n">
+      <c r="I16" s="1" t="n">
         <v>1.3799</v>
       </c>
-      <c r="J16" s="5" t="n">
+      <c r="J16" s="1" t="n">
         <v>-1.6436</v>
       </c>
-      <c r="K16" s="5" t="n">
+      <c r="K16" s="1" t="n">
         <v>-0.5111</v>
       </c>
-      <c r="L16" s="5" t="n">
+      <c r="L16" s="1" t="n">
         <v>-1.0852</v>
       </c>
-      <c r="M16" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4021,7 +4016,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4031,49 +4026,49 @@
       <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="n">
+      <c r="B1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="n">
+      <c r="C1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="D1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="n">
+      <c r="E1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="n">
+      <c r="F1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="G1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="n">
+      <c r="H1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I1" s="4" t="n">
+      <c r="I1" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="J1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="K1" s="4" t="n">
+      <c r="K1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="L1" s="4" t="n">
+      <c r="L1" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="M1" s="4" t="n">
+      <c r="M1" s="3" t="n">
         <v>60</v>
       </c>
       <c r="N1" s="3"/>
@@ -4082,40 +4077,40 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="1" t="n">
         <v>-0.558</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="1" t="n">
         <v>-0.313</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="1" t="n">
         <v>-0.0886</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="1" t="n">
         <v>0.5674</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="1" t="n">
         <v>-0.448</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="1" t="n">
         <v>-0.4768</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="1" t="n">
         <v>-0.598</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="1" t="n">
         <v>-0.1176</v>
       </c>
-      <c r="J2" s="5" t="n">
+      <c r="J2" s="1" t="n">
         <v>-0.2783</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="K2" s="1" t="n">
         <v>-0.6083</v>
       </c>
-      <c r="L2" s="5" t="n">
+      <c r="L2" s="1" t="n">
         <v>-0.6331</v>
       </c>
-      <c r="M2" s="5" t="n">
+      <c r="M2" s="1" t="n">
         <v>0.1985</v>
       </c>
     </row>
@@ -4123,40 +4118,40 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="1" t="n">
         <v>-1.5401</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="1" t="n">
         <v>-0.0523</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="1" t="n">
         <v>-0.7026</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="1" t="n">
         <v>-0.4933</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="1" t="n">
         <v>-0.8167</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="1" t="n">
         <v>-0.0028</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="H3" s="1" t="n">
         <v>-0.6568</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="1" t="n">
         <v>-1.0267</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="J3" s="1" t="n">
         <v>-1.9867</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="K3" s="1" t="n">
         <v>-1.5253</v>
       </c>
-      <c r="L3" s="5" t="n">
+      <c r="L3" s="1" t="n">
         <v>-1.0837</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="M3" s="1" t="n">
         <v>-1.5982</v>
       </c>
     </row>
@@ -4164,40 +4159,40 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B4" s="1" t="n">
         <v>-0.3943</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="1" t="n">
         <v>3.098</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="1" t="n">
         <v>-0.7818</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.5366</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="1" t="n">
         <v>1.0477</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="1" t="n">
         <v>1.9388</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="1" t="n">
         <v>1.9985</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="1" t="n">
         <v>1.948</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="1" t="n">
         <v>2.8678</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="1" t="n">
         <v>3.26</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="1" t="n">
         <v>2.2513</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="1" t="n">
         <v>1.9187</v>
       </c>
     </row>
@@ -4205,40 +4200,40 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="1" t="n">
         <v>1.5094</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.4057</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.5999</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="1" t="n">
         <v>1.291</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="1" t="n">
         <v>1.5787</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="1" t="n">
         <v>-0.5042</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="1" t="n">
         <v>1.659</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="1" t="n">
         <v>1.728</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="1" t="n">
         <v>0.4889</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="1" t="n">
         <v>-0.2991</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="1" t="n">
         <v>0.9863</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="1" t="n">
         <v>0.9578</v>
       </c>
     </row>
@@ -4246,40 +4241,40 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="1" t="n">
         <v>-0.4169</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.6492</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="1" t="n">
         <v>-0.1259</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="1" t="n">
         <v>0.7149</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="1" t="n">
         <v>0.0457</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="1" t="n">
         <v>0.2932</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="1" t="n">
         <v>-0.3901</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="1" t="n">
         <v>0.2321</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="1" t="n">
         <v>0.9238</v>
       </c>
-      <c r="K6" s="5" t="n">
+      <c r="K6" s="1" t="n">
         <v>0.3174</v>
       </c>
-      <c r="L6" s="5" t="n">
+      <c r="L6" s="1" t="n">
         <v>-0.0252</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="1" t="n">
         <v>1.0246</v>
       </c>
     </row>
@@ -4287,40 +4282,40 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="1" t="n">
         <v>0.4102</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="1" t="n">
         <v>-0.9203</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="1" t="n">
         <v>0.3786</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="1" t="n">
         <v>-0.8169</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="1" t="n">
         <v>0.0301</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="1" t="n">
         <v>-1.4462</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="1" t="n">
         <v>-0.3025</v>
       </c>
-      <c r="I7" s="5" t="n">
+      <c r="I7" s="1" t="n">
         <v>-0.3727</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" s="1" t="n">
         <v>-0.2195</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="1" t="n">
         <v>-1.1639</v>
       </c>
-      <c r="L7" s="5" t="n">
+      <c r="L7" s="1" t="n">
         <v>0.2619</v>
       </c>
-      <c r="M7" s="5" t="n">
+      <c r="M7" s="1" t="n">
         <v>-0.5285</v>
       </c>
     </row>
@@ -4328,40 +4323,40 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="1" t="n">
         <v>2.9631</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.0054</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="1" t="n">
         <v>1.0227</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="1" t="n">
         <v>-1.8079</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="1" t="n">
         <v>2.6496</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="1" t="n">
         <v>1.8897</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="1" t="n">
         <v>1.3275</v>
       </c>
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="1" t="n">
         <v>-2.4363</v>
       </c>
-      <c r="J8" s="5" t="n">
+      <c r="J8" s="1" t="n">
         <v>1.3018</v>
       </c>
-      <c r="K8" s="5" t="n">
+      <c r="K8" s="1" t="n">
         <v>-0.2604</v>
       </c>
-      <c r="L8" s="5" t="n">
+      <c r="L8" s="1" t="n">
         <v>2.3205</v>
       </c>
-      <c r="M8" s="5" t="n">
+      <c r="M8" s="1" t="n">
         <v>-0.2676</v>
       </c>
     </row>
@@ -4369,40 +4364,40 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="1" t="n">
         <v>0.8346</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.5458</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="1" t="n">
         <v>-0.4035</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="1" t="n">
         <v>0.5827</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="1" t="n">
         <v>1.0075</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.8038</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="1" t="n">
         <v>1.1451</v>
       </c>
-      <c r="I9" s="5" t="n">
+      <c r="I9" s="1" t="n">
         <v>0.6532</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="1" t="n">
         <v>1.4213</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="1" t="n">
         <v>0.7549</v>
       </c>
-      <c r="L9" s="5" t="n">
+      <c r="L9" s="1" t="n">
         <v>0.3324</v>
       </c>
-      <c r="M9" s="5" t="n">
+      <c r="M9" s="1" t="n">
         <v>0.3404</v>
       </c>
     </row>
@@ -4410,40 +4405,40 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="1" t="n">
         <v>0.475</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.8935</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="1" t="n">
         <v>0.0344</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="1" t="n">
         <v>0.9253</v>
       </c>
-      <c r="F10" s="5" t="n">
+      <c r="F10" s="1" t="n">
         <v>-0.2822</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="1" t="n">
         <v>0.8125</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="1" t="n">
         <v>0.4466</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="1" t="n">
         <v>0.3866</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" s="1" t="n">
         <v>-0.1762</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="1" t="n">
         <v>0.4906</v>
       </c>
-      <c r="L10" s="5" t="n">
+      <c r="L10" s="1" t="n">
         <v>0.4941</v>
       </c>
-      <c r="M10" s="5" t="n">
+      <c r="M10" s="1" t="n">
         <v>0.4523</v>
       </c>
     </row>
@@ -4451,34 +4446,32 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="1" t="n">
         <v>-0.1941</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="1" t="n">
         <v>-0.1977</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="1" t="n">
         <v>0.3222</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="1" t="n">
         <v>0.4058</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="1" t="n">
         <v>-0.84</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="1" t="n">
         <v>0.4143</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="5" t="n">
+      <c r="J11" s="2"/>
+      <c r="K11" s="1" t="n">
         <v>-0.1119</v>
       </c>
-      <c r="L11" s="5" t="n">
+      <c r="L11" s="1" t="n">
         <v>0.4121</v>
       </c>
-      <c r="M11" s="5" t="n">
+      <c r="M11" s="1" t="n">
         <v>0.1617</v>
       </c>
     </row>
@@ -4486,38 +4479,37 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="1" t="n">
         <v>0.857</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.3944</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="1" t="n">
         <v>-0.0101</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="1" t="n">
         <v>-0.8563</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="1" t="n">
         <v>-0.1573</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="1" t="n">
         <v>-0.1339</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="1" t="n">
         <v>-0.1171</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="n">
+      <c r="J12" s="1" t="n">
         <v>0.3775</v>
       </c>
-      <c r="K12" s="5" t="n">
+      <c r="K12" s="1" t="n">
         <v>0.4539</v>
       </c>
-      <c r="L12" s="5" t="n">
+      <c r="L12" s="1" t="n">
         <v>0.3331</v>
       </c>
-      <c r="M12" s="5" t="n">
+      <c r="M12" s="1" t="n">
         <v>0.2096</v>
       </c>
     </row>
@@ -4525,38 +4517,37 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.1491</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="1" t="n">
         <v>-0.9615</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="1" t="n">
         <v>0.6945</v>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="1" t="n">
         <v>-1.177</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="1" t="n">
         <v>0.155</v>
       </c>
-      <c r="H13" s="5" t="n">
+      <c r="H13" s="1" t="n">
         <v>-1.3155</v>
       </c>
-      <c r="I13" s="5" t="n">
+      <c r="I13" s="1" t="n">
         <v>-0.1184</v>
       </c>
-      <c r="J13" s="5" t="n">
+      <c r="J13" s="1" t="n">
         <v>-1.0331</v>
       </c>
-      <c r="K13" s="5" t="n">
+      <c r="K13" s="1" t="n">
         <v>0.07</v>
       </c>
-      <c r="L13" s="5" t="n">
+      <c r="L13" s="1" t="n">
         <v>-0.7403</v>
       </c>
-      <c r="M13" s="5" t="n">
+      <c r="M13" s="1" t="n">
         <v>0.728</v>
       </c>
     </row>
@@ -4564,40 +4555,40 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="1" t="n">
         <v>-0.8778</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="1" t="n">
         <v>-0.5421</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="1" t="n">
         <v>-1.4449</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="1" t="n">
         <v>-0.6419</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="1" t="n">
         <v>-0.986</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="1" t="n">
         <v>-0.0224</v>
       </c>
-      <c r="H14" s="5" t="n">
+      <c r="H14" s="1" t="n">
         <v>-0.4459</v>
       </c>
-      <c r="I14" s="5" t="n">
+      <c r="I14" s="1" t="n">
         <v>-0.1383</v>
       </c>
-      <c r="J14" s="5" t="n">
+      <c r="J14" s="1" t="n">
         <v>0.9324</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="1" t="n">
         <v>1.2889</v>
       </c>
-      <c r="L14" s="5" t="n">
+      <c r="L14" s="1" t="n">
         <v>0.6571</v>
       </c>
-      <c r="M14" s="5" t="n">
+      <c r="M14" s="1" t="n">
         <v>0.9774</v>
       </c>
     </row>
@@ -4605,40 +4596,40 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="1" t="n">
         <v>-1.7099</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="1" t="n">
         <v>-1.3898</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="1" t="n">
         <v>-2.1356</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="1" t="n">
         <v>-1.6842</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="1" t="n">
         <v>-0.1238</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="1" t="n">
         <v>-1.0174</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="1" t="n">
         <v>0.37</v>
       </c>
-      <c r="I15" s="5" t="n">
+      <c r="I15" s="1" t="n">
         <v>-1.6723</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" s="1" t="n">
         <v>-0.259</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="1" t="n">
         <v>-0.2008</v>
       </c>
-      <c r="L15" s="5" t="n">
+      <c r="L15" s="1" t="n">
         <v>-1.5284</v>
       </c>
-      <c r="M15" s="5" t="n">
+      <c r="M15" s="1" t="n">
         <v>-1.0413</v>
       </c>
     </row>
@@ -4646,45 +4637,44 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="1" t="n">
         <v>-1.903</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="n">
+      <c r="D16" s="1" t="n">
         <v>1.5545</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="1" t="n">
         <v>-0.0849</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="1" t="n">
         <v>-0.6127</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="1" t="n">
         <v>1.2343</v>
       </c>
-      <c r="H16" s="5" t="n">
+      <c r="H16" s="1" t="n">
         <v>-0.5888</v>
       </c>
-      <c r="I16" s="5" t="n">
+      <c r="I16" s="1" t="n">
         <v>-0.8746</v>
       </c>
-      <c r="J16" s="5" t="n">
+      <c r="J16" s="1" t="n">
         <v>-0.8822</v>
       </c>
-      <c r="K16" s="5" t="n">
+      <c r="K16" s="1" t="n">
         <v>0.6754</v>
       </c>
-      <c r="L16" s="5" t="n">
+      <c r="L16" s="1" t="n">
         <v>-0.7341</v>
       </c>
-      <c r="M16" s="5" t="n">
+      <c r="M16" s="1" t="n">
         <v>-0.5958</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4693,7 +4683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4703,9 +4693,9 @@
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5129,26 +5119,21 @@
       <c r="C11" s="1" t="n">
         <v>0.5574</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="1" t="n">
         <v>0.297</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="1" t="n">
         <v>0.1843</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="1" t="n">
         <v>0.1582</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5" t="n">
+      <c r="J11" s="1" t="n">
         <v>1.7097</v>
       </c>
-      <c r="K11" s="5" t="n">
+      <c r="K11" s="1" t="n">
         <v>0.6198</v>
       </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -5357,8 +5342,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5367,7 +5352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5377,9 +5362,9 @@
       <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5510,7 +5495,6 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5"/>
       <c r="C4" s="1" t="n">
         <v>2.4162</v>
       </c>
@@ -5549,7 +5533,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.6693</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -5590,7 +5574,7 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="1" t="n">
         <v>0.4944</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -5631,7 +5615,7 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="1" t="n">
         <v>0.9889</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -5672,7 +5656,7 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="1" t="n">
         <v>0.3519</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -5713,7 +5697,7 @@
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="1" t="n">
         <v>-0.1455</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -5754,7 +5738,7 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="1" t="n">
         <v>0.5518</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -5781,7 +5765,7 @@
       <c r="J10" s="1" t="n">
         <v>-0.6863</v>
       </c>
-      <c r="K10" s="12" t="n">
+      <c r="K10" s="9" t="n">
         <v>0.0001</v>
       </c>
       <c r="L10" s="1" t="n">
@@ -5795,7 +5779,7 @@
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="1" t="n">
         <v>0.3316</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -5836,7 +5820,7 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="1" t="n">
         <v>-0.0389</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -5877,7 +5861,7 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="1" t="n">
         <v>-1.0275</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -5918,7 +5902,7 @@
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="n">
+      <c r="B14" s="1" t="n">
         <v>-0.7061</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -5959,7 +5943,7 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="1" t="n">
         <v>-1.7194</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -6000,7 +5984,6 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5"/>
       <c r="C16" s="1" t="n">
         <v>0.1287</v>
       </c>
@@ -6022,7 +6005,6 @@
       <c r="I16" s="1" t="n">
         <v>-0.2373</v>
       </c>
-      <c r="J16" s="5"/>
       <c r="K16" s="1" t="n">
         <v>0.6914</v>
       </c>
@@ -6035,8 +6017,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6045,7 +6027,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6055,9 +6037,9 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6862,8 +6844,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>